<commit_message>
add static and fix accept request
</commit_message>
<xml_diff>
--- a/prisma/staticfile/report_heading.xlsx
+++ b/prisma/staticfile/report_heading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work (Stream IT)\OSP\TLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27A27CD3-5892-4930-849D-16D68E44ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D73F2FC-2535-4776-AE36-7E00A855764E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21525" yWindow="4830" windowWidth="20415" windowHeight="13440" xr2:uid="{1801F8F6-CEF0-48D6-99BA-D22EDF455927}"/>
+    <workbookView xWindow="24705" yWindow="3210" windowWidth="20415" windowHeight="13440" xr2:uid="{1801F8F6-CEF0-48D6-99BA-D22EDF455927}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Certificate of Analysis</t>
+  </si>
+  <si>
+    <t>STAB</t>
+  </si>
+  <si>
+    <t>Stability Test Report</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD66A24-84C3-4E97-8EE7-F83CFE2998F9}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G8:G9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +469,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>